<commit_message>
Rebuild worldbuilder-Minecraft.py;New githubExplorer.py, Interface.cpp
</commit_message>
<xml_diff>
--- a/ODK/packList.xlsx
+++ b/ODK/packList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduNetdiskWorkspace\项目开发\奥德赛世界\程序开发\OdysseyWorld\SDK\build\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduNetdiskWorkspace\项目开发\奥德赛世界\程序开发\OdysseyWorld\ODK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5671110A-94C7-49EB-97B7-E3B554EE2264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8816036-8D41-46BE-88A4-70A7388CB51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="2080" windowWidth="19180" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2160" windowWidth="25600" windowHeight="11290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>cpp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,6 +155,42 @@
   </si>
   <si>
     <t>function module-compute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>worldBuilder-Minecraft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minecraft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a1b2c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>githubExplorer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addon module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>module只返回数据不干活</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,21 +526,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.08203125" customWidth="1"/>
+    <col min="1" max="1" width="19.9140625" customWidth="1"/>
     <col min="2" max="2" width="12.08203125" customWidth="1"/>
     <col min="3" max="3" width="43.4140625" customWidth="1"/>
     <col min="4" max="5" width="17.58203125" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="7" max="7" width="14.58203125" customWidth="1"/>
+    <col min="7" max="7" width="21.58203125" customWidth="1"/>
     <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -532,7 +569,9 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -641,6 +680,66 @@
       </c>
       <c r="H6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>